<commit_message>
Further translations from map 102 and 104
</commit_message>
<xml_diff>
--- a/data/Map102.xlsx
+++ b/data/Map102.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="395">
   <si>
     <t>自動実行</t>
   </si>
@@ -49,10 +49,21 @@
 どうやって外に・・・鉄格子は！？</t>
   </si>
   <si>
+    <t>\n&lt;ロメリア&gt;Ehh!?
+Alsy!?
+That was an iron cell...how did you get out!?</t>
+  </si>
+  <si>
     <t>開いてた</t>
   </si>
   <si>
+    <t>It opened.</t>
+  </si>
+  <si>
     <t>擦ったら摩擦で溶けた</t>
+  </si>
+  <si>
+    <t>I rubbed it really hard and it melted.</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;嘘！
@@ -60,21 +71,41 @@
 ラッキー・・・！</t>
   </si>
   <si>
+    <t>\n&lt;ロメリア&gt;You're joking!
+No way...they forgot to lock it!?
+What a stroke of luck...!</t>
+  </si>
+  <si>
     <t>\n&lt;ロメリア&gt;いや、待って。怪しい・・・
 罠かもしれない。気を付けてあにき。
 あいつら、何か企んでるのかも。</t>
   </si>
   <si>
+    <t>\n&lt;ロメリア&gt;No, wait. That's too suspicious...
+It might be a trap. You should be careful Alsy,
+they could be plotting something.</t>
+  </si>
+  <si>
     <t>\n&lt;ロメリア&gt;あれだけ搾られた癖に冗談言うなんて余裕あるね。
 さすがあにき。
 死んどけ。</t>
   </si>
   <si>
+    <t>\n&lt;ロメリア&gt;They've been draining you so much, and yet
+you can still crack a joke huh? That's my big brother!
+Still standing!</t>
+  </si>
+  <si>
     <t>\n&lt;ロメリア&gt;でもこんなに簡単に出られるなんてなんか怪しくない？
 気を付けて。
 罠かもしれないよ。</t>
   </si>
   <si>
+    <t>\n&lt;ロメリア&gt;But don't you think it's weird you could just get out?
+Be careful.
+It might be some kind of trap.</t>
+  </si>
+  <si>
     <t>MP_SET_MOVIE アルス立ち絵アニメ基本</t>
   </si>
   <si>
@@ -82,7 +113,7 @@
 どうやって出たんだ！？</t>
   </si>
   <si>
-    <t xml:space="preserve">
+    <t>\n&lt;アルス&gt;Wha, you...!
 How did you get out!?</t>
   </si>
   <si>
@@ -97,17 +128,35 @@
 これはチャンスだぞ！</t>
   </si>
   <si>
+    <t>\n&lt;アルス&gt;Could they have forgotten to lock the cell...?
+T-This is it!
+This could be our big break!</t>
+  </si>
+  <si>
     <t>\n&lt;アルス&gt;いや待て。何か怪しいな・・・
 こんなに簡単に獲物を逃がすか？
 罠かもしれないぞ。気を付けろ。\n[1]。</t>
   </si>
   <si>
+    <t>\n&lt;アルス&gt;Wait. Something is off...
+Could escaping really be that easy?
+This could be a trap. Be careful, \n[1].</t>
+  </si>
+  <si>
     <t>\n&lt;アルス&gt;まさか俺の妹がゴリラだったなんてな。
 すまん、この鉄格子も頼む。</t>
   </si>
   <si>
+    <t>\n&lt;アルス&gt;I had no idea my littler sister was a gorilla!
+I hope you don't mind if I trouble you to do this cell too.</t>
+  </si>
+  <si>
     <t>\n&lt;アルス&gt;どうやら俺の鉄格子はお前のところより固いようだな。
 サビていたのか・・・？</t>
+  </si>
+  <si>
+    <t>\n&lt;アルス&gt;Ah, it seems like the bars of my cell are a bit
+tougher. Were yours rusty...?</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;こんなに簡単に出られるのは逆に怪しいな。
@@ -115,6 +164,11 @@
 気を付けろ。\n[1]。</t>
   </si>
   <si>
+    <t>\n&lt;アルス&gt;Being able to get out so easily is suspicious indeed.
+It could be a trap.
+Be careful, \n[1].</t>
+  </si>
+  <si>
     <t>\n&lt;リリー&gt;鍵を掛けたかどうか不安な時って結局
 ほとんどの場合はちゃんと鍵掛けてるのよね。
 無意識にっていうか。</t>
@@ -299,6 +353,9 @@
     <t>鉄格子は硬く閉ざされている・・・</t>
   </si>
   <si>
+    <t>The iron bars have been securely fastened...</t>
+  </si>
+  <si>
     <t>EV005</t>
   </si>
   <si>
@@ -306,11 +363,19 @@
 あいつらにやられたのだろうか・・・</t>
   </si>
   <si>
+    <t>A corpse can be seen inside...
+Did those guys really...?</t>
+  </si>
+  <si>
     <t>しかばね</t>
   </si>
   <si>
     <t>返事がない・・・
 ただの屍のようだ・・・</t>
+  </si>
+  <si>
+    <t>There is no response...
+It seems to be just a dead body...</t>
   </si>
   <si>
     <t>ロメ/アル</t>
@@ -434,6 +499,11 @@
 If you die on your own, I'll kill you-nya.</t>
   </si>
   <si>
+    <t>\n&lt;Shina&gt;Huuh?
+But I was next-nya...
+You better not kill him, or I'll kill you too-nya!</t>
+  </si>
+  <si>
     <t>\n&lt;リリー&gt;ちょっと、次はライムの番よ。
 しれっと順番抜かしてるんじゃないわよ。
 ライム、おいで。</t>
@@ -444,6 +514,11 @@
 Come on Lime.</t>
   </si>
   <si>
+    <t>\n&lt;Lily&gt;Now now, next is Lime's turn.
+Order is very important you know.
+Come on Lime.</t>
+  </si>
+  <si>
     <t>\n&lt;ライム&gt;んん・・・！！</t>
   </si>
   <si>
@@ -456,6 +531,10 @@
   <si>
     <t>\n&lt;Shina&gt;Tch...
 Make them cum quickly then-nya.</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Tch...
+Alright, just make him spurt quickly-nya.</t>
   </si>
   <si>
     <t>\n&lt;リリー&gt;どーお？ライム、美味しい？</t>
@@ -484,6 +563,11 @@
 My hand is all slippery-nya.</t>
   </si>
   <si>
+    <t>\n&lt;Shina&gt;I can feel it getting really slimy too.
+Nyaha-
+My hand is all slippery-nya.</t>
+  </si>
+  <si>
     <t>\n&lt;ライム&gt;んぁっ♥
 ん・・・♥
 ごく・・・ごく・・・♥</t>
@@ -520,6 +604,11 @@
 And now they fainted.</t>
   </si>
   <si>
+    <t>\n&lt;Lime&gt;Mm...paah~
+Sorry. I think I sucked too hard.
+And now they fainted.</t>
+  </si>
+  <si>
     <t>\n&lt;シィナ&gt;にゃぁ！！
 次アタシにゃぁ！！
 アタシだったのにゃぁー！！</t>
@@ -834,14 +923,28 @@
 屈辱だ・・・</t>
   </si>
   <si>
+    <t>Being forced to wear this prison uniform...
+How humiliating...</t>
+  </si>
+  <si>
     <t>※イベント中の立ち絵アニメの表示を設定します。
 （オプションでいつでも変更可能です）</t>
   </si>
   <si>
+    <t>※Here, you can set if main character is seen during events.
+(You may also change this in the options menu at any time.)</t>
+  </si>
+  <si>
     <t>立ち絵アニメをON</t>
   </si>
   <si>
+    <t>Display the main character</t>
+  </si>
+  <si>
     <t>立ち絵アニメをOFF</t>
+  </si>
+  <si>
+    <t>Do not display the main character</t>
   </si>
   <si>
     <t>立ち絵アニメを表示するようにしました。
@@ -849,23 +952,44 @@
 ※一部の攻撃は立ち絵アニメが自動で非表示になります。</t>
   </si>
   <si>
+    <t>The main character will now be displayed during events.
+※If it is hiding enemy attacks, change it in the options menu.
+※Some enemy attacks will hide the main character by default.</t>
+  </si>
+  <si>
     <t>立ち絵アニメを非表示にしました。</t>
   </si>
   <si>
+    <t>The main character will not be displayed.</t>
+  </si>
+  <si>
     <t>変更しませんでした。</t>
   </si>
   <si>
+    <t>No change was made.</t>
+  </si>
+  <si>
     <t>今は鏡を見ている場合じゃない！</t>
   </si>
   <si>
+    <t>This is no time to watch yourself in the mirror!</t>
+  </si>
+  <si>
     <t>タル</t>
   </si>
   <si>
     <t>中身は空っぽだ・・・</t>
+  </si>
+  <si>
+    <t>It's completely empty...</t>
   </si>
   <si>
     <t>・・・！
 よし、この中なら隠れられそうだ！</t>
+  </si>
+  <si>
+    <t>...!
+That's right, this would be the perfect hiding spot!</t>
   </si>
   <si>
     <t>\n&lt;リリー&gt;・・・</t>
@@ -998,6 +1122,9 @@
     <t>一応飲めそうな水・・・</t>
   </si>
   <si>
+    <t>Water suitable for drinking...</t>
+  </si>
+  <si>
     <t>この水を全部飲み干して桶を被れば・・・！！</t>
   </si>
   <si>
@@ -1105,7 +1232,13 @@
     <t>まずはあにきに話しかけよう・・・</t>
   </si>
   <si>
+    <t>I should talk to Alsy first...</t>
+  </si>
+  <si>
     <t>まずはロメリアに話しかけよう・・・</t>
+  </si>
+  <si>
+    <t>I should speak with Romelia first...</t>
   </si>
   <si>
     <t>EV022</t>
@@ -1823,1811 +1956,2018 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>58</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>63</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="D49" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>65</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>66</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+      <c r="D52" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>69</v>
+      </c>
+      <c r="D54" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>70</v>
+      </c>
+      <c r="D55" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>71</v>
+      </c>
+      <c r="D56" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="D59" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="D60" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="D61" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>77</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="D63" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>80</v>
+      </c>
+      <c r="D65" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="D67" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>86</v>
+      </c>
+      <c r="D69" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D72" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D73" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D82" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B83" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D83" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D84" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D85" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D86" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D87" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D88" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B89" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D89" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D90" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="D91" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B92" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="D92" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="B93" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D93" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="D94" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B95" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="D95" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B96" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="D96" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="B97" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="D97" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B98" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="D98" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B99" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="D99" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="B100" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="D100" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B101" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D101" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="B102" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="D102" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="D103" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B104" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D104" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="B105" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D105" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B106" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="D106" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="B107" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="D107" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="B109" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="D109" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B110" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="D110" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D111" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B112" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="D112" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="B113" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="D113" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="B114" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="D114" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="B115" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="D115" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="B116" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="D116" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B117" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D117" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B118" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D118" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="B119" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="D119" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="B120" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="D120" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="B121" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="D121" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="B122" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="D122" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B123" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D123" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="B124" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="D124" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B125" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="D125" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B126" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="D126" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B127" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D127" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="B128" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D128" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B129" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="D129" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="B130" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="D130" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B131" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="D131" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>218</v>
+      </c>
+      <c r="D141" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>199</v>
+        <v>220</v>
+      </c>
+      <c r="D142" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>200</v>
+        <v>222</v>
+      </c>
+      <c r="D143" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>201</v>
+        <v>224</v>
+      </c>
+      <c r="D144" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>202</v>
+        <v>226</v>
+      </c>
+      <c r="D145" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>203</v>
+        <v>228</v>
+      </c>
+      <c r="D146" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>204</v>
+        <v>230</v>
+      </c>
+      <c r="D147" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>205</v>
+        <v>232</v>
+      </c>
+      <c r="D148" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>207</v>
+        <v>235</v>
+      </c>
+      <c r="D150" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>208</v>
+        <v>237</v>
+      </c>
+      <c r="D151" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>212</v>
+        <v>242</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>213</v>
+        <v>243</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>218</v>
+        <v>248</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>220</v>
+        <v>250</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>221</v>
+        <v>251</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>244</v>
+        <v>274</v>
+      </c>
+      <c r="D187" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
       <c r="D192" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="D193" t="s">
-        <v>252</v>
+        <v>283</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>253</v>
+        <v>284</v>
       </c>
       <c r="D194" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="C195" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="C196" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="C197" t="s">
-        <v>260</v>
+        <v>291</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>261</v>
+        <v>292</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>264</v>
+        <v>295</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>269</v>
+        <v>300</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>271</v>
+        <v>302</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>273</v>
+        <v>304</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>274</v>
+        <v>305</v>
+      </c>
+      <c r="D211" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>275</v>
+        <v>307</v>
+      </c>
+      <c r="D212" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>276</v>
+        <v>309</v>
       </c>
       <c r="B213" t="s">
-        <v>276</v>
+        <v>309</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>277</v>
+        <v>310</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>278</v>
+        <v>311</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>279</v>
+        <v>312</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>283</v>
+        <v>316</v>
       </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>284</v>
+        <v>317</v>
       </c>
       <c r="B221" t="s">
-        <v>284</v>
+        <v>317</v>
       </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>285</v>
+        <v>318</v>
       </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>286</v>
+        <v>319</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>287</v>
+        <v>320</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>288</v>
+        <v>321</v>
       </c>
       <c r="B225" t="s">
-        <v>288</v>
+        <v>321</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>289</v>
+        <v>322</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>290</v>
+        <v>323</v>
       </c>
       <c r="B227" t="s">
-        <v>291</v>
-      </c>
-      <c r="C227" t="s">
-        <v>292</v>
+        <v>324</v>
+      </c>
+      <c r="D227" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>293</v>
+        <v>326</v>
       </c>
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>294</v>
+        <v>327</v>
       </c>
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>295</v>
+        <v>328</v>
       </c>
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>296</v>
+        <v>329</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>298</v>
+        <v>331</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>299</v>
+        <v>332</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>300</v>
+        <v>333</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>302</v>
+        <v>335</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>303</v>
+        <v>336</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>306</v>
+        <v>339</v>
       </c>
       <c r="B241" t="s">
-        <v>306</v>
+        <v>339</v>
       </c>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>307</v>
+        <v>340</v>
       </c>
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>308</v>
+        <v>341</v>
       </c>
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>309</v>
+        <v>342</v>
       </c>
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>310</v>
+        <v>343</v>
       </c>
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>311</v>
+        <v>344</v>
       </c>
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>312</v>
+        <v>345</v>
       </c>
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>313</v>
+        <v>346</v>
       </c>
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>315</v>
+        <v>348</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>317</v>
+        <v>350</v>
       </c>
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>318</v>
+        <v>351</v>
       </c>
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>319</v>
+        <v>352</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>320</v>
+        <v>353</v>
       </c>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>321</v>
+        <v>354</v>
       </c>
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>322</v>
+        <v>355</v>
       </c>
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>323</v>
+        <v>356</v>
       </c>
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>324</v>
+        <v>357</v>
       </c>
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>325</v>
+        <v>358</v>
       </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>327</v>
+        <v>360</v>
       </c>
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>328</v>
+        <v>361</v>
       </c>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>329</v>
+        <v>362</v>
       </c>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>330</v>
+        <v>363</v>
       </c>
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>332</v>
+        <v>365</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>334</v>
+        <v>367</v>
       </c>
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>336</v>
+        <v>369</v>
       </c>
       <c r="B271" t="s">
-        <v>336</v>
+        <v>369</v>
       </c>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>337</v>
+        <v>370</v>
       </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>338</v>
+        <v>371</v>
       </c>
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>339</v>
+        <v>372</v>
       </c>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>340</v>
+        <v>373</v>
       </c>
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>341</v>
+        <v>374</v>
       </c>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>342</v>
+        <v>375</v>
       </c>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>343</v>
+        <v>376</v>
       </c>
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>344</v>
+        <v>377</v>
       </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
       <c r="B280" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>346</v>
+        <v>379</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>348</v>
+        <v>381</v>
       </c>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>349</v>
+        <v>382</v>
       </c>
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>351</v>
+        <v>384</v>
       </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>352</v>
+        <v>385</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>354</v>
+        <v>387</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>355</v>
+        <v>388</v>
       </c>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>356</v>
+        <v>389</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>357</v>
+        <v>390</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>358</v>
+        <v>391</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" t="s">
-        <v>359</v>
+        <v>392</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" t="s">
-        <v>360</v>
+        <v>393</v>
       </c>
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>361</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Translation Updates to Map.102
</commit_message>
<xml_diff>
--- a/data/Map102.xlsx
+++ b/data/Map102.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="476">
   <si>
     <t>自動実行</t>
   </si>
@@ -178,15 +178,15 @@
 無意識にっていうか。</t>
   </si>
   <si>
-    <t>\n&lt;Lily&gt;鍵を掛けたかどうか不安な時って結局
-ほとんどの場合はちゃんと鍵掛けてるのよね。
-無意識にっていうか。</t>
+    <t>\n&lt;Lily&gt;You know, when someone is concerned they forgot to shut a door,
+there's a 99% chance they closed it to begin with.
+It's like a subconscious thing.</t>
   </si>
   <si>
     <t>\n&lt;ライム&gt;あるあるー。</t>
   </si>
   <si>
-    <t>\n&lt;Lime&gt;あるあるー。</t>
+    <t>\n&lt;Lime&gt;Such is the way of life-.</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;まずい！あいつらだ！
@@ -194,9 +194,9 @@
 どこか隠れられる場所はないか！？</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;まずい！あいつらだ！
-戻って来た！
-どこか隠れられる場所はないか！？</t>
+    <t>\n&lt;Als&gt;Not good! It's them!
+They've come back!
+Is there some place you can hide!?</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;あいつらの声・・・！！
@@ -204,17 +204,17 @@
 どうしようあにき！隠れられる場所とか・・・！</t>
   </si>
   <si>
-    <t>\n&lt;Romelia&gt;あいつらの声・・・！！
-戻って来た！！
-どうしようあにき！隠れられる場所とか・・・！</t>
+    <t>\n&lt;Romelia&gt;Those voices...!!
+They're coming back!!
+What do we do Alsy! There must be somewhere you can hide...!</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;早く隠れろ！
 どこか・・・なんかあるだろ！</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;早く隠れろ！
-どこか・・・なんかあるだろ！</t>
+    <t>\n&lt;Als&gt;Hide, on the double!
+There must be somewhere around!</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;見つかる前に隠れて！
@@ -222,9 +222,9 @@
 急いで！</t>
   </si>
   <si>
-    <t>\n&lt;Romelia&gt;見つかる前に隠れて！
-早く！
-急いで！</t>
+    <t>\n&lt;Romelia&gt;Hide before they spot you!
+Quickly!
+And hurry!</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;・・・
@@ -232,9 +232,9 @@
 なんか妙なことになったな。</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;・・・
-聞こえてたか？
-なんか妙なことになったな。</t>
+    <t>\n&lt;Als&gt;...
+Did you hear that?
+Now that was weird.</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;だけど、これはチャンスでもある。
@@ -242,9 +242,9 @@
 脱出経路を探すんだ。</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;だけど、これはチャンスでもある。
-あいつらが調子に乗って油断しているうちに
-脱出経路を探すんだ。</t>
+    <t>\n&lt;Als&gt;But, this could be our big chance.
+It's the perfect time to search for an escape route
+while they're caught up in the moment.</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;\n[1]。もし逃げられるようなら
@@ -252,23 +252,29 @@
 分かったな？</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;\n[1]。もし逃げられるようなら
-俺の事は気にせず逃げるんだぞ。
-分かったな？</t>
+    <t>\n&lt;Als&gt;\n[1]. If you are able to run away, 
+then do so. Do not worry about me.
+Do you understand?</t>
   </si>
   <si>
     <t>置いてはいけない</t>
   </si>
   <si>
+    <t>Don't say things like that.</t>
+  </si>
+  <si>
     <t>うん</t>
+  </si>
+  <si>
+    <t>I understand.</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;俺のことは大丈夫だ。
 お前さえ無事なら・・・</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;俺のことは大丈夫だ。
-お前さえ無事なら・・・</t>
+    <t>\n&lt;Als&gt;I will be just fine.
+As long as you are safe...</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;少し距離はあるが、無事に逃げ延びたら
@@ -276,9 +282,9 @@
 それまでの間くらい、耐えてみせるさ。</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;少し距離はあるが、無事に逃げ延びたら
-ギルドに行って助けを呼んできてくれ。
-それまでの間くらい、耐えてみせるさ。</t>
+    <t>\n&lt;Als&gt;Although it is a little far from here, there is
+a nearby guild you can call on for help.
+Until then, I'll be waiting.</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;よし。
@@ -286,27 +292,31 @@
 あまり無茶はするな。</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;よし。
-気を付けて行けよ。\n[1]。
-あまり無茶はするな。</t>
+    <t>\n&lt;Als&gt;That's it.
+Be careful, \n[1].
+Don't do anything rash.</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;ぐぅ～・・・・（腹の鳴る音）</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;ぐぅ～・・・・（腹の鳴る音）</t>
+    <t>\n&lt;Als&gt;*Gurgle...* (You can hear their belly rumble)</t>
   </si>
   <si>
     <t>\n&lt;\n[1]&gt;あにき、お腹鳴ってるよ。
 何か食べ物があったら持ってくるね。</t>
   </si>
   <si>
+    <t>\n&lt;\n[1]&gt;Alsy, I can hear your stomach groaning.
+I'll bring back some food for you, okay?</t>
+  </si>
+  <si>
     <t>\n&lt;アルス&gt;う・・・悪い。
 余裕があったらでいいぞ。</t>
   </si>
   <si>
-    <t>\n&lt;Als&gt;う・・・悪い。
-余裕があったらでいいぞ。</t>
+    <t>\n&lt;Als&gt;I'm...fine.
+There is no need to rush yourself for me.</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;なんか変なことになったね。
@@ -314,9 +324,9 @@
 まぁ、ある意味チャンスだけど。</t>
   </si>
   <si>
-    <t>\n&lt;Romelia&gt;なんか変なことになったね。
-脱出ゲーム・・・
-まぁ、ある意味チャンスだけど。</t>
+    <t>\n&lt;Romelia&gt;That was kind of weird wasn't it?
+An escape game...
+Well, this could be a big chance for us though.</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;あの三馬鹿が調子に乗っているうちに
@@ -324,15 +334,15 @@
 あにき、頑張れ！</t>
   </si>
   <si>
-    <t>\n&lt;Romelia&gt;あの三馬鹿が調子に乗っているうちに
-なんとかここを抜け出す方法を探そう！
-あにき、頑張れ！</t>
+    <t>\n&lt;Romelia&gt;You might be able to look for some way out
+while those three idiots are distracted!
+Do your best, Alsy!</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;ぐぅ～・・・（お腹の鳴る音）</t>
   </si>
   <si>
-    <t>\n&lt;Romelia&gt;ぐぅ～・・・（お腹の鳴る音）</t>
+    <t>\n&lt;Romelia&gt;*Groan...* (You can hear their stomach growling)</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;あ、ごめん。
@@ -340,9 +350,9 @@
 お、お腹空きすぎて・・・</t>
   </si>
   <si>
-    <t>\n&lt;Romelia&gt;あ、ごめん。
-何か食べるものあったらお願いできる？
-お、お腹空きすぎて・・・</t>
+    <t>\n&lt;Romelia&gt;Ah, sorry about that.
+Could I ask you to get something to eat when you go?
+M-My stomach is killing me...</t>
   </si>
   <si>
     <t>\C[3]※SAN値（正気度）について
@@ -350,20 +360,27 @@
 SAN値によって発生するイベントが変わります。</t>
   </si>
   <si>
+    <t>\C[3]※Sanity Level Explaination:
+\C[0]If you are caught and milked, your mind can become lost in pleasure.
+During these events, your sanity level will change.</t>
+  </si>
+  <si>
     <t>SAN値はお菓子を見つけてアルスに渡すことで回復します。
 現在のSAN値はアイテムの手鏡で確認できます。（初期値10）</t>
   </si>
   <si>
-    <t>SAN値はお菓子を見つけてAlsに渡すことで回復します。
-現在のSAN値はアイテムの手鏡で確認できます。（初期値10）</t>
+    <t>Sanity levels can be recovered by finding snacks and sharing them with Als.
+Your current sanity can be checked by using the Hand Mirror in your items list.
+(Sanity is initially set to 10)</t>
   </si>
   <si>
     <t>SAN値はお菓子を見つけてロメリアに渡すことで回復します。
 現在のSAN値はアイテムの手鏡で確認できます。（初期値10）</t>
   </si>
   <si>
-    <t>SAN値はお菓子を見つけてRomeliaに渡すことで回復します。
-現在のSAN値はアイテムの手鏡で確認できます。（初期値10）</t>
+    <t>Sanity levels can be recovered by finding snacks and sharing them with Romelia.
+Your current sanity can be checked by using the Hand Mirror in your items list.
+(Sanity is initially set to 10)</t>
   </si>
   <si>
     <t>\n&lt;アルス&gt;うーん。
@@ -536,6 +553,9 @@
 兄貴までこんなことになって・・・</t>
   </si>
   <si>
+    <t>\n&lt;ロメリア&gt;ごめんね。</t>
+  </si>
+  <si>
     <t>気にするな</t>
   </si>
   <si>
@@ -650,6 +670,11 @@
 If you die on your own, I'll kill you-nya.</t>
   </si>
   <si>
+    <t>\n&lt;Shina&gt;Huuh?
+I was next-nya...
+If you kill him, I'll kill you-nya.</t>
+  </si>
+  <si>
     <t>\n&lt;リリー&gt;ちょっと、次はライムの番よ。
 しれっと順番抜かしてるんじゃないわよ。
 ライム、おいで。</t>
@@ -700,6 +725,10 @@
 My hand is all slippery-nya.</t>
   </si>
   <si>
+    <t>\n&lt;Shina&gt;It feels all slimy too. Nyaha!
+My hand is all slippery-nya.</t>
+  </si>
+  <si>
     <t>\n&lt;ライム&gt;んぁっ♥
 ん・・・♥
 ごく・・・ごく・・・♥</t>
@@ -736,6 +765,11 @@
 And now they fainted.</t>
   </si>
   <si>
+    <t>\n&lt;Lime&gt;Pahh...
+Sorry. I think I sucked too hard.
+And now they fainted.</t>
+  </si>
+  <si>
     <t>\n&lt;シィナ&gt;にゃぁ！！
 次アタシにゃぁ！！
 アタシだったのにゃぁー！！</t>
@@ -812,6 +846,9 @@
     <t>\n&lt;Romeria&gt; This way!</t>
   </si>
   <si>
+    <t>\n&lt;Romeria&gt;This way!</t>
+  </si>
+  <si>
     <t>最初のイベ</t>
   </si>
   <si>
@@ -1843,7 +1880,7 @@
 苦痛などの描写はありません。</t>
   </si>
   <si>
-    <t>To note, acts of digestion are always accompanied by pleasure.
+    <t>Furthermore, acts of digestion are always accompanied by pleasure.
 There are no descriptions of pain or suffering.</t>
   </si>
 </sst>
@@ -2444,2005 +2481,2008 @@
         <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D51" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D54" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D55" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D56" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D57" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D61" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D62" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C64" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D64" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D65" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D66" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D67" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D69" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>122</v>
+        <v>126</v>
+      </c>
+      <c r="D71" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B72" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D72" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B73" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D73" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B82" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B83" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D83" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D85" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D86" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B87" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D87" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B88" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D88" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B89" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D89" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B90" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D90" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B91" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D91" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B92" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D92" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B93" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D93" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B94" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D94" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D95" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D96" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B97" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D97" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D99" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B100" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D100" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B101" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D101" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B102" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D102" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D103" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D104" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D105" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D106" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D107" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B109" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D109" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="D110" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D111" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="B112" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D112" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="B113" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D113" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D114" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B115" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="D115" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="B116" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="D116" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B117" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="D117" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="D118" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="B119" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D119" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B120" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D120" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B121" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D121" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B122" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D122" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B123" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D123" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B124" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="D124" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B125" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D125" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B126" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="D126" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B127" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="D127" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="B128" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D128" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="B129" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="D129" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B130" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="D130" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B131" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="D131" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="D141" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D142" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="D143" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="D144" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="D145" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="D146" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="D147" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D148" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="D150" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="D151" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="D152" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="D153" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="D154" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="D155" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="D156" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="D157" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="D158" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="D159" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="D160" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="D161" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="D162" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="D163" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="D164" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="D165" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="D166" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="D167" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="D168" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="D169" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="D170" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D171" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="D172" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="D173" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="D174" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="D175" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="D176" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="D177" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="D178" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="D179" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D180" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="D181" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="D182" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="D183" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D184" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="D185" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="D187" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="D192" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="D193" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D194" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="C195" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="D195" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="C196" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="D196" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="C197" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="D197" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="D211" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="D212" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="B213" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="D213" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="B221" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="D221" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="B225" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="D225" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="B227" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C227" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="D227" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="D228" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D229" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="D230" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="B241" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="D241" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="B271" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="D271" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="D272" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="B280" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="D280" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="D281" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="D289" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="D290" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="D291" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="D292" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="D293" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="D294" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="D295" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="D296" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>